<commit_message>
Notificaciones v1 y algunos cambios
</commit_message>
<xml_diff>
--- a/Otros documentos/TAREAS_USUARIOS_SIGAB.xlsx
+++ b/Otros documentos/TAREAS_USUARIOS_SIGAB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Documents\GitHub\SIGAB\Otros documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Documentos\GitHub\SIGAB\Otros documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE1433-05AD-4E6E-8313-9E20D4867FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB1B07E-BF62-4C2E-8ACF-215A27CAFBD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,14 +524,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -540,6 +534,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -554,11 +554,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -844,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,33 +878,33 @@
     <row r="2" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -933,10 +930,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -962,10 +959,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -991,10 +988,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1020,10 +1017,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1049,10 +1046,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1078,10 +1075,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1107,10 +1104,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1136,10 +1133,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1165,10 +1162,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1194,10 +1191,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1223,10 +1220,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1252,10 +1249,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1281,10 +1278,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1310,10 +1307,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1339,10 +1336,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1368,10 +1365,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -1397,10 +1394,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1426,10 +1423,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1455,10 +1452,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1484,10 +1481,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1509,10 +1506,10 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1532,10 +1529,10 @@
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1557,10 +1554,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1582,10 +1579,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -1607,10 +1604,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -1632,10 +1629,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1657,10 +1654,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1680,10 +1677,10 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1705,20 +1702,20 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="13" t="s">
+      <c r="D32" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G32" s="3"/>
@@ -1728,20 +1725,20 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="13" t="s">
+      <c r="D33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G33" s="3"/>
@@ -1751,20 +1748,20 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="13" t="s">
+      <c r="D34" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G34" s="3"/>
@@ -1774,20 +1771,20 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="13" t="s">
+      <c r="D35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G35" s="3"/>
@@ -1797,20 +1794,20 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" s="13" t="s">
+      <c r="D36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G36" s="3"/>
@@ -1820,20 +1817,20 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="13" t="s">
+      <c r="D37" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="3"/>
@@ -1843,18 +1840,18 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="9" t="s">
+      <c r="E38" s="12"/>
+      <c r="F38" s="19" t="s">
         <v>69</v>
       </c>
       <c r="G38" s="3"/>
@@ -1864,18 +1861,18 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="9" t="s">
+      <c r="E39" s="12"/>
+      <c r="F39" s="19" t="s">
         <v>69</v>
       </c>
       <c r="G39" s="3"/>
@@ -1885,18 +1882,16 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12" t="s">
+      <c r="C40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G40" s="2"/>
@@ -1906,18 +1901,16 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12" t="s">
+      <c r="C41" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>69</v>
       </c>
       <c r="G41" s="2"/>

</xml_diff>